<commit_message>
Vectors length now goes from 100 to 5000000
</commit_message>
<xml_diff>
--- a/Time_Template.xlsx
+++ b/Time_Template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesco\Desktop\ASD_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D29108-4879-4C29-8C61-D26AAF14899A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE425B59-7B66-4482-84B3-41E078AB1596}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="10" sheetId="1" r:id="rId1"/>
+    <sheet name="100" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -544,7 +546,7 @@
   <dimension ref="A1:S54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>

</xml_diff>